<commit_message>
Subiendo "agregar_archivo" modificando todo
</commit_message>
<xml_diff>
--- a/codigos/wb7.xlsx
+++ b/codigos/wb7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sara Palacios\Documents\SaraUR\Programación\proyecto2\proyecto_final_prog\codigos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{921C3AD7-C60C-4D97-A7A6-79C0F848D080}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AEC34EE-96CA-4AF2-82AC-69CEDC1D2137}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="47">
   <si>
     <t>TIPO DE PRODUCTO</t>
   </si>
@@ -95,9 +95,6 @@
   </si>
   <si>
     <t>5g</t>
-  </si>
-  <si>
-    <t>15 mg</t>
   </si>
   <si>
     <t>10g</t>
@@ -516,7 +513,7 @@
   <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,22 +619,22 @@
         <v>24</v>
       </c>
       <c r="I2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J2" t="s">
         <v>25</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>26</v>
       </c>
-      <c r="K2" t="s">
-        <v>27</v>
-      </c>
       <c r="L2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O2" s="1">
         <v>0</v>
@@ -660,43 +657,43 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
         <v>28</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>29</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>30</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>31</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>32</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>33</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>34</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>35</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>36</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" t="s">
+        <v>36</v>
+      </c>
+      <c r="N3" t="s">
         <v>37</v>
-      </c>
-      <c r="L3" t="s">
-        <v>27</v>
-      </c>
-      <c r="M3" t="s">
-        <v>37</v>
-      </c>
-      <c r="N3" t="s">
-        <v>38</v>
       </c>
       <c r="O3" s="1">
         <v>0.25</v>
@@ -719,43 +716,43 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
         <v>39</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>40</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>41</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" t="s">
         <v>42</v>
-      </c>
-      <c r="F4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" t="s">
-        <v>43</v>
       </c>
       <c r="H4" t="s">
         <v>24</v>
       </c>
       <c r="I4" t="s">
+        <v>43</v>
+      </c>
+      <c r="J4" t="s">
         <v>44</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>45</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M4" t="s">
+        <v>26</v>
+      </c>
+      <c r="N4" t="s">
         <v>46</v>
-      </c>
-      <c r="L4" t="s">
-        <v>27</v>
-      </c>
-      <c r="M4" t="s">
-        <v>27</v>
-      </c>
-      <c r="N4" t="s">
-        <v>47</v>
       </c>
       <c r="O4" s="1">
         <v>0.02</v>

</xml_diff>